<commit_message>
Added more NPCs and Enemies
</commit_message>
<xml_diff>
--- a/01_ProjectPlanning/pmSheet.xlsx
+++ b/01_ProjectPlanning/pmSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NITRO\Desktop\HTL\Programmieren\Project\if.05.61_01-project-repository\01_ProjectPlanning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NITRO\Desktop\KingdomOfSouls\01_ProjectPlanning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF1497F-02F6-4672-BE0B-D8CAD9903088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD13E70F-E340-4D7E-BA89-42DEE674EB65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4F780517-EDF3-40DE-9578-A00B65031757}"/>
+    <workbookView xWindow="2460" yWindow="3240" windowWidth="21600" windowHeight="11385" xr2:uid="{4F780517-EDF3-40DE-9578-A00B65031757}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>Writing the Story</t>
   </si>
   <si>
-    <t>Implement enemies</t>
-  </si>
-  <si>
     <t>Implement attacks</t>
   </si>
   <si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>&gt; Implement Combo/Partner Attack Mechanic</t>
+  </si>
+  <si>
+    <t>Implement enemies/npcs</t>
   </si>
 </sst>
 </file>
@@ -462,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B7A473B-8019-4D26-B2B4-6F04769690C4}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +502,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1">
         <v>15</v>
@@ -518,12 +518,12 @@
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1">
         <v>10</v>
@@ -539,12 +539,12 @@
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1">
         <v>5</v>
@@ -560,12 +560,12 @@
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
         <v>8</v>
@@ -581,12 +581,12 @@
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1">
         <v>10</v>
@@ -602,12 +602,12 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1">
         <v>12</v>
@@ -623,7 +623,7 @@
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -668,12 +668,12 @@
         <v>4</v>
       </c>
       <c r="F13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="1">
         <v>15</v>
@@ -682,19 +682,19 @@
         <v>15</v>
       </c>
       <c r="D14" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B15" s="1">
         <v>15</v>
@@ -703,19 +703,19 @@
         <v>15</v>
       </c>
       <c r="D15" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1">
         <v>20</v>
@@ -731,12 +731,12 @@
         <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1">
         <v>15</v>
@@ -752,7 +752,7 @@
         <v>15</v>
       </c>
       <c r="F17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -763,7 +763,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -772,7 +772,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1">
         <v>20</v>
@@ -788,12 +788,12 @@
         <v>20</v>
       </c>
       <c r="F20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1">
         <v>20</v>
@@ -809,12 +809,12 @@
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1">
         <v>20</v>
@@ -830,12 +830,12 @@
         <v>20</v>
       </c>
       <c r="F22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1">
         <v>15</v>
@@ -851,7 +851,7 @@
         <v>15</v>
       </c>
       <c r="F23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More Battle System Core Mechanics, did some adjustements for attacks and thought a little more about the story -> how map looks like
</commit_message>
<xml_diff>
--- a/01_ProjectPlanning/pmSheet.xlsx
+++ b/01_ProjectPlanning/pmSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NITRO\Desktop\KingdomOfSouls\01_ProjectPlanning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BFE491-AC5F-48E0-B29D-A426E40810AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2BA535-29B6-4DE3-8454-7DA79FA3682E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{4F780517-EDF3-40DE-9578-A00B65031757}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4F780517-EDF3-40DE-9578-A00B65031757}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -463,7 +463,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,11 +511,11 @@
         <v>20</v>
       </c>
       <c r="D3" s="1">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1">
         <f>C3-D3</f>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -661,11 +661,11 @@
         <v>6</v>
       </c>
       <c r="D13" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" t="s">
         <v>9</v>
@@ -682,11 +682,11 @@
         <v>15</v>
       </c>
       <c r="D14" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
messed up alot. will try do fix all later
</commit_message>
<xml_diff>
--- a/01_ProjectPlanning/pmSheet.xlsx
+++ b/01_ProjectPlanning/pmSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NITRO\Desktop\KingdomOfSouls\01_ProjectPlanning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2BA535-29B6-4DE3-8454-7DA79FA3682E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA871AC5-87B0-4EC8-8CED-B21FDC0F4AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4F780517-EDF3-40DE-9578-A00B65031757}"/>
   </bookViews>
@@ -463,7 +463,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,11 +511,11 @@
         <v>20</v>
       </c>
       <c r="D3" s="1">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1">
         <f>C3-D3</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>

</xml_diff>